<commit_message>
basic version done, row-based env setup done
</commit_message>
<xml_diff>
--- a/simulation_data/latency.xlsx
+++ b/simulation_data/latency.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EB26B6-887F-4843-8C0F-04E9D82716A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6A8EDB-DEEB-4225-975C-F6BCD54F0CBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CONV1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FC3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:E7"/>
+  <dimension ref="C4:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -380,7 +392,7 @@
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -390,8 +402,17 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -401,13 +422,22 @@
       <c r="E5">
         <v>1011</v>
       </c>
+      <c r="F5">
+        <v>181</v>
+      </c>
+      <c r="G5">
+        <v>39</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
ADD row based CONV1 and CONV2
</commit_message>
<xml_diff>
--- a/simulation_data/latency.xlsx
+++ b/simulation_data/latency.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6A8EDB-DEEB-4225-975C-F6BCD54F0CBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2ECF45-F92F-4CFC-BDD6-47D0EB914FAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="C4:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -436,6 +436,12 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>42</v>
+      </c>
+      <c r="E6">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">

</xml_diff>

<commit_message>
add single core version
</commit_message>
<xml_diff>
--- a/simulation_data/latency.xlsx
+++ b/simulation_data/latency.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761DCE2-5919-4212-A070-766EC0186FDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE9E999-54D1-4BA0-B403-0B447441CFC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>CONV1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,18 +34,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Systolic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Base</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ms</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>FC1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -55,6 +47,22 @@
   </si>
   <si>
     <t>FC3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-cores</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>single-cores</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>us</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -380,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:H7"/>
+  <dimension ref="C3:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -392,9 +400,14 @@
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -403,49 +416,136 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>1461</v>
+        <v>1860292</v>
       </c>
       <c r="E5">
-        <v>1011</v>
+        <v>1300248</v>
       </c>
       <c r="F5">
-        <v>181</v>
+        <v>215341</v>
       </c>
       <c r="G5">
-        <v>39</v>
+        <v>45394</v>
       </c>
       <c r="H5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+        <v>4761</v>
+      </c>
+      <c r="I5">
+        <v>3424721</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>42</v>
+        <v>542124</v>
       </c>
       <c r="E6">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+        <v>59945</v>
+      </c>
+      <c r="F6">
+        <v>121786</v>
+      </c>
+      <c r="G6">
+        <v>26239</v>
+      </c>
+      <c r="H6">
+        <v>3313</v>
+      </c>
+      <c r="I6">
+        <v>262148</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>3</v>
+      </c>
+      <c r="D11">
+        <v>1461003</v>
+      </c>
+      <c r="E11">
+        <v>1010759</v>
+      </c>
+      <c r="F11">
+        <v>180305</v>
+      </c>
+      <c r="G11">
+        <v>38025</v>
+      </c>
+      <c r="H11">
+        <v>3941</v>
+      </c>
+      <c r="I11">
+        <v>2693829</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>42052</v>
+      </c>
+      <c r="E12">
+        <v>46022</v>
+      </c>
+      <c r="F12">
+        <v>97821</v>
+      </c>
+      <c r="G12">
+        <v>20799</v>
+      </c>
+      <c r="H12">
+        <v>2808</v>
+      </c>
+      <c r="I12">
+        <v>209361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add report and readme
</commit_message>
<xml_diff>
--- a/simulation_data/latency.xlsx
+++ b/simulation_data/latency.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1546A298-3A44-41D9-AA64-4CAD84D0C0F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88424CE-E537-4865-AA20-11FBD93D16FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
   <si>
     <t>CONV1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,14 @@
   </si>
   <si>
     <t>Actual total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HLS latency cimparison without Bus latency</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -782,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:J28"/>
+  <dimension ref="C2:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -899,7 +907,7 @@
         <v>97</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" ref="E7:I7" si="0">100-ROUND(E6/E5,2)*100</f>
+        <f t="shared" ref="E7:H7" si="0">100-ROUND(E6/E5,2)*100</f>
         <v>95</v>
       </c>
       <c r="F7" s="4">
@@ -1301,6 +1309,167 @@
         <v>20</v>
       </c>
     </row>
+    <row r="30" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="16">
+        <v>14194</v>
+      </c>
+      <c r="E33" s="1">
+        <v>9628</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1924</v>
+      </c>
+      <c r="G33" s="1">
+        <v>406</v>
+      </c>
+      <c r="H33" s="1">
+        <v>34</v>
+      </c>
+      <c r="I33" s="2">
+        <v>262148</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="16">
+        <v>4667</v>
+      </c>
+      <c r="E34" s="1">
+        <v>3641</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1941</v>
+      </c>
+      <c r="G34" s="1">
+        <v>512</v>
+      </c>
+      <c r="H34" s="1">
+        <v>46</v>
+      </c>
+      <c r="I34" s="2">
+        <v>209361</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="3">
+        <f>100-ROUND(D34/D33,2)*100</f>
+        <v>67</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" ref="E35:I35" si="14">100-ROUND(E34/E33,2)*100</f>
+        <v>62</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="14"/>
+        <v>-1</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" si="14"/>
+        <v>-26</v>
+      </c>
+      <c r="H35" s="25">
+        <f t="shared" si="14"/>
+        <v>-35</v>
+      </c>
+      <c r="I35" s="5">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="6"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="24"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="7"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="21"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="7"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="21"/>
+    </row>
+    <row r="41" spans="3:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="8"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>